<commit_message>
added 2020 4th quarter data to program.
</commit_message>
<xml_diff>
--- a/data/jobGrowthByQuarter.xlsx
+++ b/data/jobGrowthByQuarter.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr fullCalcOnLoad="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Year &amp; Quarter</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>2020-Q3</t>
+  </si>
+  <si>
+    <t>2020-Q4</t>
   </si>
 </sst>
 </file>
@@ -531,8 +534,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xr:uid="{434e80c3-331c-4145-a0cf-8c336655a10a}">
-  <dimension ref="A1:B24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0e738be4-24db-4753-9ea2-e05ef2333a79}">
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
@@ -551,7 +554,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>405</v>
+        <v>418</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12.75">
@@ -567,7 +570,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12.75">
@@ -575,7 +578,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12.75">
@@ -583,7 +586,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>777</v>
+        <v>778</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="12.75">
@@ -591,7 +594,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="12.75">
@@ -599,7 +602,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="1">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="12.75">
@@ -607,7 +610,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="1">
-        <v>188</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="12.75">
@@ -615,7 +618,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="1">
-        <v>1094</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="12.75">
@@ -623,7 +626,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="1">
-        <v>218</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="12.75">
@@ -631,7 +634,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="1">
-        <v>181</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="12.75">
@@ -639,7 +642,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="1">
-        <v>275</v>
+        <v>291</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12.75">
@@ -647,7 +650,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="1">
-        <v>1925</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="12.75">
@@ -655,7 +658,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="1">
-        <v>351</v>
+        <v>364</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="12.75">
@@ -663,7 +666,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="1">
-        <v>376</v>
+        <v>392</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12.75">
@@ -671,7 +674,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="1">
-        <v>361</v>
+        <v>369</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="12.75">
@@ -687,7 +690,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="1">
-        <v>560</v>
+        <v>573</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="12.75">
@@ -695,7 +698,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="1">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="12.75">
@@ -703,7 +706,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="1">
-        <v>632</v>
+        <v>621</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="12.75">
@@ -711,7 +714,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="1">
-        <v>1610</v>
+        <v>1685</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="12.75">
@@ -719,7 +722,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="1">
-        <v>1352</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="12.75">
@@ -727,7 +730,15 @@
         <v>24</v>
       </c>
       <c r="B24" s="1">
-        <v>576</v>
+        <v>639</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="12.75">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="1">
+        <v>542</v>
       </c>
     </row>
   </sheetData>
@@ -741,18 +752,18 @@
 	 "version" : 1,
 	 "reportServers": [
 		{
-		  "id": "277c1529-5ec7-11eb-bfd2-e2ca7635a565",
+		  "id": "1ada6e8b-90c1-11eb-aad2-5a030a9abb45",
 		  "name": "",
 		  "description": "",
 		  "url": "https://d7qphkkvookir94.us.qlikcloud.com/api/v1/reports",
 		  "webIntegrationId": "",
 		  "reportApps": [
 			{
-			  "id": "277c152d-5ec7-11eb-bfd2-e2ca7635a565",
+			  "id": "1ada6e8d-90c1-11eb-aad2-5a030a9abb45",
 			  "name": "App from reporting-service",
 			  "description": "App",
 			  "sourceAppId": "d21fa1b4-0aef-4d99-96ee-02dac1b09ece",
-			  "appReloadTime": "2021-01-14T01:22:10Z"
+			  "appReloadTime": "2021-03-29T18:35:03Z"
         	}
 		 ]
     	}
@@ -761,13 +772,13 @@
 		{
 		  "isDetached": false,
 		  "properties": [],
-	      "id": "277c152f-5ec7-11eb-bfd2-e2ca7635a565",
+	      "id": "1ada6e8f-90c1-11eb-aad2-5a030a9abb45",
     	  "name": "Table",
 	      "description": "table",
 	      "type": "table",
-	      "key": "table_277c152f5ec711ebbfd2e2ca7635a565",
-	      "serverId": "277c1529-5ec7-11eb-bfd2-e2ca7635a565",
-	      "appId": "277c152d-5ec7-11eb-bfd2-e2ca7635a565",
+	      "key": "table_1ada6e8f90c111ebaad25a030a9abb45",
+	      "serverId": "1ada6e8b-90c1-11eb-aad2-5a030a9abb45",
+	      "appId": "1ada6e8d-90c1-11eb-aad2-5a030a9abb45",
 	      "entityId": "upHawrQ",
 		  "selections": []
 	    }

</xml_diff>